<commit_message>
ONEDEVOPS-126 API TEST CASES
</commit_message>
<xml_diff>
--- a/PlatformRegressionTest/src/main/resources/Test_Data.xlsx
+++ b/PlatformRegressionTest/src/main/resources/Test_Data.xlsx
@@ -9,21 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AgentRegistration" sheetId="1" r:id="rId1"/>
     <sheet name="UpdateAgent" sheetId="2" r:id="rId2"/>
     <sheet name="DeleteAgent" sheetId="3" r:id="rId3"/>
     <sheet name="SaveCorrelation" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId5"/>
-    <sheet name="UpdateCorrelation" sheetId="7" r:id="rId6"/>
-    <sheet name="DeleteCorrelation" sheetId="8" r:id="rId7"/>
-    <sheet name="AddUser" sheetId="9" r:id="rId8"/>
-    <sheet name="UpdateUser" sheetId="10" r:id="rId9"/>
-    <sheet name="AssignUser" sheetId="11" r:id="rId10"/>
-    <sheet name="SaveWebhook" sheetId="13" r:id="rId11"/>
-    <sheet name="Sheet3" sheetId="14" r:id="rId12"/>
+    <sheet name="UpdateCorrelation" sheetId="7" r:id="rId5"/>
+    <sheet name="DeleteCorrelation" sheetId="8" r:id="rId6"/>
+    <sheet name="AddUser" sheetId="9" r:id="rId7"/>
+    <sheet name="UpdateUser" sheetId="10" r:id="rId8"/>
+    <sheet name="AssignUser" sheetId="11" r:id="rId9"/>
+    <sheet name="SaveWebhook" sheetId="13" r:id="rId10"/>
+    <sheet name="Sheet3" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -47,144 +46,6 @@
   </si>
   <si>
     <t xml:space="preserve">configJson </t>
-  </si>
-  <si>
-    <t>{
-   "vault":{
-      "getFromVault":false,
-      "secretEngine":"insights-kv",
-      "readToken":"vault_secret_token",
-      "vaultUrl":"http://Vault_Host:port/v1/"
-   },
-   "mqConfig":{
-      "user":"iSight",
-      "password":"iSight",
-      "host":"127.0.0.1",
-      "exchange":"iSight",
-      "agentControlXchg":"iAgent"
-   },
-   "enrichData":{
-      "isEnrichmentRequired":true,
-      "sourceProperty":"message",
-      "keyPattern":"-",
-      "targetProperty":"key"
-   },
-   "subscribe":{
-      "config":"SCM.GIT.config"
-   },
-   "publish":{
-      "data":"SCM.GIT.DATA",
-      "health":"SCM.GIT.HEALTH"
-   },
-   "communication":{
-      "type":"REST",
-      "sslVerify":false,
-      "responseType":"JSON"
-   },
-   "dynamicTemplate":{
-      "timeFieldMapping":{
-         "startDate":"%Y-%m-%d",
-         "createdAt":"%Y-%m-%dT%H:%M:%SZ",
-         "updatedAt":"%Y-%m-%dT%H:%M:%SZ",
-         "closedAt":"%Y-%m-%dT%H:%M:%SZ",
-         "mergedAt":"%Y-%m-%dT%H:%M:%SZ",
-         "commitTime":"%Y-%m-%dT%H:%M:%SZ",
-         "since":"%Y-%m-%dT%H:%M:%SZ",
-         "until":"%Y-%m-%dT%H:%M:%SZ",
-         "consumptionTime":"%Y-%m-%dT%H:%M:%SZ"
-      },
-      "responseTemplate":{
-         "sha":"commitId",
-         "commit":{
-            "message":"message",
-            "author":{
-               "name":"authorName",
-               "date":"commitTime"
-            }
-         }
-      },
-      "pullReqResponseTemplate":{
-         "number":"pullReqId",
-         "state":"pullReqState",
-         "head":{
-            "sha":"headSHA",
-            "ref":"originBranch",
-            "repo":{
-               "fork":"isForked"
-            }
-         },
-         "base":{
-            "sha":"baseSHA",
-            "ref":"baseBranch"
-         },
-         "isMerged":"isMerged",
-         "originBranchJiraKeys":"originBranchJiraKeys",
-         "merge_commit_sha":"mergedSHA",
-         "commit":"commit",
-         "created_at":"createdAt",
-         "updated_at":"updatedAt",
-         "closed_at":"closedAt",
-         "merged_at":"mergedAt"
-      },
-      "metaData":{
-         "branches":{
-            "dataUpdateSupported":true,
-            "uniqueKey":[
-               "repoName",
-               "gitType"
-            ]
-         },
-         "pullRequest":{
-            "dataUpdateSupported":true,
-            "uniqueKey":[
-               "repoName",
-               "pullReqId",
-               "gitType"
-            ]
-         },
-         "commits":{
-            "dataUpdateSupported":true,
-            "uniqueKey":[
-               "repoName",
-               "commitId",
-               "gitType"
-            ]
-         }
-      }
-   },
-   "agentId":"git_api_test",
-   "enableBranches":true,
-   "enableOptimizedDataRetrieval":true,
-   "enablePullReqCommitAPIDataRetrieval":true,
-   "enableBrancheDeletion":false,
-   "enableDataValidation":true,
-   "toolCategory":"SCM",
-   "toolsTimeZone":"GMT",
-   "insightsTimeZone":"Asia/Kolkata",
-   "enableValueArray":false,
-   "useResponseTemplate":true,
-   "auth":"base64",
-   "runSchedule":30,
-   "timeStampField":"commitTime",
-   "timeStampFormat":"%Y-%m-%dT%H:%M:%SZ",
-   "agentSecretDetails":[
-      "accessToken"
-   ],
-   "isEpochTimeFormat":false,
-   "startFrom":"2017-10-01 00:00:01",
-   "accessToken":"accessToken",
-   "getRepos":null,
-   "commitsBaseEndPoint":null,
-   "isDebugAllowed":false,
-   "loggingSetting":{
-      "logLevel":"WARN",
-      "maxBytes":5000000,
-      "backupCount":1000
-   }
-}</t>
-  </si>
-  <si>
-    <t>windows</t>
   </si>
   <si>
     <t>v6.5</t>
@@ -580,6 +441,144 @@
   </si>
   <si>
     <t>pvt_webhook_test</t>
+  </si>
+  <si>
+    <t>{
+   "vault":{
+      "getFromVault":false,
+      "secretEngine":"insights-kv",
+      "readToken":"vault_secret_token",
+      "vaultUrl":"http://Vault_Host:port/v1/"
+   },
+   "mqConfig":{
+      "user":"iSight",
+      "password":"iSight",
+      "host":"127.0.0.1",
+      "exchange":"iSight",
+      "agentControlXchg":"iAgent"
+   },
+   "enrichData":{
+      "isEnrichmentRequired":true,
+      "sourceProperty":"message",
+      "keyPattern":"-",
+      "targetProperty":"key"
+   },
+   "subscribe":{
+      "config":"SCM.GIT.config"
+   },
+   "publish":{
+      "data":"SCM.GIT_API.DATA",
+      "health":"SCM.GIT_API.HEALTH"
+   },
+   "communication":{
+      "type":"REST",
+      "sslVerify":false,
+      "responseType":"JSON"
+   },
+   "dynamicTemplate":{
+      "timeFieldMapping":{
+         "startDate":"%Y-%m-%d",
+         "createdAt":"%Y-%m-%dT%H:%M:%SZ",
+         "updatedAt":"%Y-%m-%dT%H:%M:%SZ",
+         "closedAt":"%Y-%m-%dT%H:%M:%SZ",
+         "mergedAt":"%Y-%m-%dT%H:%M:%SZ",
+         "commitTime":"%Y-%m-%dT%H:%M:%SZ",
+         "since":"%Y-%m-%dT%H:%M:%SZ",
+         "until":"%Y-%m-%dT%H:%M:%SZ",
+         "consumptionTime":"%Y-%m-%dT%H:%M:%SZ"
+      },
+      "responseTemplate":{
+         "sha":"commitId",
+         "commit":{
+            "message":"message",
+            "author":{
+               "name":"authorName",
+               "date":"commitTime"
+            }
+         }
+      },
+      "pullReqResponseTemplate":{
+         "number":"pullReqId",
+         "state":"pullReqState",
+         "head":{
+            "sha":"headSHA",
+            "ref":"originBranch",
+            "repo":{
+               "fork":"isForked"
+            }
+         },
+         "base":{
+            "sha":"baseSHA",
+            "ref":"baseBranch"
+         },
+         "isMerged":"isMerged",
+         "originBranchJiraKeys":"originBranchJiraKeys",
+         "merge_commit_sha":"mergedSHA",
+         "commit":"commit",
+         "created_at":"createdAt",
+         "updated_at":"updatedAt",
+         "closed_at":"closedAt",
+         "merged_at":"mergedAt"
+      },
+      "metaData":{
+         "branches":{
+            "dataUpdateSupported":true,
+            "uniqueKey":[
+               "repoName",
+               "gitType"
+            ]
+         },
+         "pullRequest":{
+            "dataUpdateSupported":true,
+            "uniqueKey":[
+               "repoName",
+               "pullReqId",
+               "gitType"
+            ]
+         },
+         "commits":{
+            "dataUpdateSupported":true,
+            "uniqueKey":[
+               "repoName",
+               "commitId",
+               "gitType"
+            ]
+         }
+      }
+   },
+   "agentId":"git_api_test",
+   "enableBranches":true,
+   "enableOptimizedDataRetrieval":true,
+   "enablePullReqCommitAPIDataRetrieval":true,
+   "enableBrancheDeletion":false,
+   "enableDataValidation":true,
+   "toolCategory":"SCM",
+   "toolsTimeZone":"GMT",
+   "insightsTimeZone":"Asia/Kolkata",
+   "enableValueArray":false,
+   "useResponseTemplate":true,
+   "auth":"base64",
+   "runSchedule":30,
+   "timeStampField":"commitTime",
+   "timeStampFormat":"%Y-%m-%dT%H:%M:%SZ",
+   "agentSecretDetails":[
+      "accessToken"
+   ],
+   "isEpochTimeFormat":false,
+   "startFrom":"2017-10-01 00:00:01",
+   "accessToken":"580abc475eba19ee6c17a0f93c93858e7bf80b96",
+   "getRepos":"https://api.github.com/users/poojagupta285/repos",
+   "commitsBaseEndPoint":"https://api.github.com/repos/poojagupta285/",
+   "isDebugAllowed":false,
+   "loggingSetting":{
+      "logLevel":"WARN",
+      "maxBytes":5000000,
+      "backupCount":1000
+   }
+}</t>
+  </si>
+  <si>
+    <t>windows</t>
   </si>
 </sst>
 </file>
@@ -931,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -958,21 +957,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="b">
         <v>0</v>
@@ -986,57 +985,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1">
-        <v>755790</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1064,93 +1015,93 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
         <v>58</v>
       </c>
-      <c r="L1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
       <c r="O1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K2">
         <v>-1</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -1171,75 +1122,75 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>66</v>
       </c>
       <c r="K1">
         <v>-1</v>
       </c>
       <c r="L1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N1" t="b">
         <v>1</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>76</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -1248,54 +1199,54 @@
         <v>-1</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N3" t="b">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
         <v>64</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
       </c>
       <c r="K5">
         <v>-1</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" t="b">
@@ -1304,40 +1255,40 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
         <v>64</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>66</v>
       </c>
       <c r="K6">
         <v>-1</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" t="b">
@@ -1355,14 +1306,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1377,24 +1331,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -1411,37 +1365,37 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1472,51 +1426,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>0</v>
@@ -1529,19 +1483,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1557,15 +1498,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1577,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1592,12 +1533,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1606,12 +1547,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,48 +1563,86 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C2" s="1">
         <v>755790</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1674,34 +1653,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="1">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="D2" s="1">
+        <v>755790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insights Release 8.2 changes
</commit_message>
<xml_diff>
--- a/PlatformRegressionTest/src/main/resources/Test_Data.xlsx
+++ b/PlatformRegressionTest/src/main/resources/Test_Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\842100\OneDrive - Cognizant\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\841870\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8E572D-8B7D-40E2-8EAB-761545E4F48C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="AgentRegistration" sheetId="1" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
   <si>
     <t>toolName</t>
   </si>
@@ -570,16 +569,13 @@
     <t>john@microsoft.com</t>
   </si>
   <si>
-    <t>v8.0</t>
-  </si>
-  <si>
     <t>GIT_TO_GIT_APITEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -922,23 +918,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="4" max="4" width="42.08984375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,12 +951,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>70</v>
@@ -979,33 +975,33 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="34.90625" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" customWidth="1"/>
-    <col min="11" max="11" width="5.6328125" customWidth="1"/>
-    <col min="12" max="12" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.36328125" customWidth="1"/>
-    <col min="15" max="15" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1048,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1106,20 +1102,20 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1166,7 +1162,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1210,7 +1206,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1301,19 +1297,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1333,7 +1329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1360,16 +1356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1404,26 +1400,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +1445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1469,7 +1465,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>0</v>
@@ -1482,20 +1478,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1503,9 +1499,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -1518,26 +1514,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1547,21 +1543,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1584,7 +1580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1609,7 +1605,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B6DA136D-1488-4B49-89D0-51B1FA2B028E}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1617,16 +1613,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1637,7 +1633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1655,20 +1651,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1682,7 +1678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>